<commit_message>
add scroll-behavior:smooth; & tweak
</commit_message>
<xml_diff>
--- a/document/portfolio画面構成図.xlsx
+++ b/document/portfolio画面構成図.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/016f3f629cf49fa7/ドキュメント/WebPages/Portfolio/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{307FF492-3586-473C-9D4F-5CDF58BC23F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DE959194-48A8-4F70-9F0A-8A44958A8567}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{307FF492-3586-473C-9D4F-5CDF58BC23F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63DB0923-3888-4EE9-81B7-AA5E65B9DA4F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9CAB5321-B9DA-419D-9B26-BFE33E30EA37}"/>
+    <workbookView xWindow="2530" yWindow="290" windowWidth="12090" windowHeight="10510" xr2:uid="{9CAB5321-B9DA-419D-9B26-BFE33E30EA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,11 +91,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:colOff>431800</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="10714215" cy="5529527"/>
+    <xdr:ext cx="12573000" cy="8777146"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="16" name="テキスト ボックス 15">
@@ -109,8 +109,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7594600" y="6400800"/>
-          <a:ext cx="10714215" cy="5529527"/>
+          <a:off x="7696200" y="6400800"/>
+          <a:ext cx="12573000" cy="8777146"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -132,7 +132,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -140,6 +140,81 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
             <a:t>ドロップダウンはスクロールせず固定させたい</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+            <a:t>(2020/10/30 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
+            <a:t>実装済</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
+            <a:t>サブメニューはドロップダウン</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>デフォルトで</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>実装済</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
         </a:p>
@@ -149,7 +224,175 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
-            <a:t>サブメニューはドロップダウン</a:t>
+            <a:t>ハッシュでコンテンツに飛ばすページ内遷移</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="3200">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(2020/10/30 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>実装済</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)(2020/10/31 scroll-behavior:smooth;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>追加</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="3200">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
+            <a:t>コンテンツは</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+            <a:t>iframe</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
+            <a:t>で表示し、クリックで画面遷移させる</a:t>
+          </a:r>
+          <a:endParaRPr lang="ja-JP" altLang="ja-JP" sz="3200">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>実現できるが、実装見送り</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2020/10/30</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
         </a:p>
@@ -159,36 +402,20 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
-            <a:t>ハッシュでコンテンツに飛ばすページ内遷移</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+            <a:t>スクロールの裏に画像入れたい</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
-            <a:t>コンテンツは</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
-            <a:t>iframe</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
-            <a:t>で表示し、クリックで画面遷移させる</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
-            <a:t>スクロールの裏に画像入れたい</a:t>
-          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1183,7 +1410,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34488283-59BF-46F7-BC37-89B7764A758F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AO56" sqref="AO56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>

</xml_diff>

<commit_message>
fix border gradient and effect to emulate
</commit_message>
<xml_diff>
--- a/document/portfolio画面構成図.xlsx
+++ b/document/portfolio画面構成図.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Portfolio\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Products\Portfolio\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F57B669-05C3-4E79-855E-2F2E2C2DD3F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390B812-15F2-4089-B484-FD1412A504F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2530" yWindow="290" windowWidth="12090" windowHeight="10510" xr2:uid="{9CAB5321-B9DA-419D-9B26-BFE33E30EA37}"/>
+    <workbookView xWindow="7310" yWindow="290" windowWidth="11740" windowHeight="10510" xr2:uid="{9CAB5321-B9DA-419D-9B26-BFE33E30EA37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,18 +179,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>(</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>デフォルトで</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="3200">
@@ -1410,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34488283-59BF-46F7-BC37-89B7764A758F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AK31" sqref="AK31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>